<commit_message>
Added Occupancy and ARR Charts in Excel File
</commit_message>
<xml_diff>
--- a/PythonScripts/Exponential Triple Smoothing Experiment - Copy.xlsx
+++ b/PythonScripts/Exponential Triple Smoothing Experiment - Copy.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jade Ericson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jade Ericson\Documents\GitHub\Revenue-Forecaster\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>alpha</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>factor</t>
+  </si>
+  <si>
+    <t>occupancy</t>
+  </si>
+  <si>
+    <t>arr</t>
   </si>
 </sst>
 </file>
@@ -608,7 +614,805 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$7:$R$42</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CFB6-4A4E-9C43-516A9F77F95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="485749648"/>
+        <c:axId val="485750304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="485749648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485750304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="485750304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485749648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$7:$S$42</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>4196</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3840</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3530</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3715</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3585</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3420</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3757</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3480</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3713</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3885</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4723</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4146</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4065</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4765</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4648</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4328</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4143</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3954</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4035</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4122</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4380</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5169</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4727</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4534</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4608</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4647</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4744</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4292</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4349</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4297</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4516</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5544</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E305-4091-B578-44962E626CD7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="399086760"/>
+        <c:axId val="399088072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="399086760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399088072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="399088072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="399086760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1164,6 +1968,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1197,6 +3033,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0B9CFE8-E611-4602-991A-FFF271CE128E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>200186</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>178230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>145295</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64576</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBBB812C-56C4-4898-B6CE-990040480588}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1502,10 +3410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5994F0-3FF4-479C-8EA5-B8061AF23392}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7:S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,10 +3422,14 @@
     <col min="3" max="3" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="8"/>
     <col min="6" max="6" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="7" max="17" width="9.140625" style="8"/>
+    <col min="18" max="18" width="12.42578125" style="8" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +3437,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1533,7 +3445,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1541,7 +3453,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1553,7 +3465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1572,8 +3484,14 @@
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="R6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -1589,8 +3507,14 @@
         <f>C7-AVERAGE($C$7:$C$18)</f>
         <v>3257275.8585148249</v>
       </c>
+      <c r="R7" s="8">
+        <v>55</v>
+      </c>
+      <c r="S7" s="8">
+        <v>4196</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f>A7+1</f>
         <v>2</v>
@@ -1608,8 +3532,14 @@
         <f>C8-AVERAGE($C$7:$C$18)</f>
         <v>-1074940.9179458171</v>
       </c>
+      <c r="R8" s="8">
+        <v>51</v>
+      </c>
+      <c r="S8" s="8">
+        <v>3840</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f t="shared" ref="A9:A18" si="0">A8+1</f>
         <v>3</v>
@@ -1624,11 +3554,17 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6">
-        <f t="shared" ref="F9:F19" si="2">C9-AVERAGE($C$7:$C$18)</f>
+        <f t="shared" ref="F9:F18" si="2">C9-AVERAGE($C$7:$C$18)</f>
         <v>576570.12473047338</v>
       </c>
+      <c r="R9" s="8">
+        <v>56</v>
+      </c>
+      <c r="S9" s="8">
+        <v>3530</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1646,8 +3582,14 @@
         <f t="shared" si="2"/>
         <v>3635419.4608475026</v>
       </c>
+      <c r="R10" s="8">
+        <v>65</v>
+      </c>
+      <c r="S10" s="8">
+        <v>3715</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1665,8 +3607,14 @@
         <f t="shared" si="2"/>
         <v>1803230.8597508203</v>
       </c>
+      <c r="R11" s="8">
+        <v>59</v>
+      </c>
+      <c r="S11" s="8">
+        <v>3585</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1684,8 +3632,14 @@
         <f t="shared" si="2"/>
         <v>-2262415.6289851777</v>
       </c>
+      <c r="R12" s="8">
+        <v>49</v>
+      </c>
+      <c r="S12" s="8">
+        <v>3420</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1703,8 +3657,14 @@
         <f t="shared" si="2"/>
         <v>-8652335.8663111757</v>
       </c>
+      <c r="R13" s="8">
+        <v>24</v>
+      </c>
+      <c r="S13" s="8">
+        <v>3438</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1722,8 +3682,14 @@
         <f t="shared" si="2"/>
         <v>-9650176.5962851755</v>
       </c>
+      <c r="R14" s="8">
+        <v>19</v>
+      </c>
+      <c r="S14" s="8">
+        <v>3757</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1741,8 +3707,14 @@
         <f t="shared" si="2"/>
         <v>-5533469.1301141363</v>
       </c>
+      <c r="R15" s="8">
+        <v>36</v>
+      </c>
+      <c r="S15" s="8">
+        <v>3480</v>
+      </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <f>A15+1</f>
         <v>10</v>
@@ -1760,8 +3732,14 @@
         <f t="shared" si="2"/>
         <v>455397.39927586354</v>
       </c>
+      <c r="R16" s="8">
+        <v>52</v>
+      </c>
+      <c r="S16" s="8">
+        <v>3713</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1779,8 +3757,14 @@
         <f t="shared" si="2"/>
         <v>5661030.5676148217</v>
       </c>
+      <c r="R17" s="8">
+        <v>69</v>
+      </c>
+      <c r="S17" s="8">
+        <v>3885</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1803,8 +3787,14 @@
         <f t="shared" si="2"/>
         <v>11784413.868907185</v>
       </c>
+      <c r="R18" s="8">
+        <v>71</v>
+      </c>
+      <c r="S18" s="8">
+        <v>4723</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1</v>
       </c>
@@ -1827,8 +3817,14 @@
         <f>$B$3*(C19-D19)+(1-$B$3)*(F7)</f>
         <v>3472166.7716988255</v>
       </c>
+      <c r="R19" s="8">
+        <v>63</v>
+      </c>
+      <c r="S19" s="8">
+        <v>4146</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <f>A19+1</f>
         <v>2</v>
@@ -1852,8 +3848,14 @@
         <f t="shared" ref="F20:F41" si="5">$B$3*(C20-D20)+(1-$B$3)*(F8)</f>
         <v>-968944.11375024635</v>
       </c>
+      <c r="R20" s="8">
+        <v>58</v>
+      </c>
+      <c r="S20" s="8">
+        <v>4065</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <f t="shared" ref="A21:A30" si="6">A20+1</f>
         <v>3</v>
@@ -1877,8 +3879,14 @@
         <f t="shared" si="5"/>
         <v>610897.12309943093</v>
       </c>
+      <c r="R21" s="8">
+        <v>50</v>
+      </c>
+      <c r="S21" s="8">
+        <v>4765</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -1902,8 +3910,14 @@
         <f t="shared" si="5"/>
         <v>3383818.6616325979</v>
       </c>
+      <c r="R22" s="8">
+        <v>53</v>
+      </c>
+      <c r="S22" s="8">
+        <v>4648</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -1927,8 +3941,14 @@
         <f t="shared" si="5"/>
         <v>2000111.5747197508</v>
       </c>
+      <c r="R23" s="8">
+        <v>60</v>
+      </c>
+      <c r="S23" s="8">
+        <v>4328</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -1952,8 +3972,14 @@
         <f t="shared" si="5"/>
         <v>-2501018.1722823502</v>
       </c>
+      <c r="R24" s="8">
+        <v>42</v>
+      </c>
+      <c r="S24" s="8">
+        <v>4143</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -1977,8 +4003,14 @@
         <f t="shared" si="5"/>
         <v>-7930473.5832310598</v>
       </c>
+      <c r="R25" s="8">
+        <v>52</v>
+      </c>
+      <c r="S25" s="8">
+        <v>3954</v>
+      </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -2002,8 +4034,14 @@
         <f t="shared" si="5"/>
         <v>-9315189.0645949896</v>
       </c>
+      <c r="R26" s="8">
+        <v>53</v>
+      </c>
+      <c r="S26" s="8">
+        <v>4050</v>
+      </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -2027,8 +4065,14 @@
         <f t="shared" si="5"/>
         <v>-6100262.6487604072</v>
       </c>
+      <c r="R27" s="8">
+        <v>45</v>
+      </c>
+      <c r="S27" s="8">
+        <v>4035</v>
+      </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <f>A27+1</f>
         <v>10</v>
@@ -2052,8 +4096,14 @@
         <f t="shared" si="5"/>
         <v>-181278.94992776029</v>
       </c>
+      <c r="R28" s="8">
+        <v>47</v>
+      </c>
+      <c r="S28" s="8">
+        <v>4122</v>
+      </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -2077,8 +4127,14 @@
         <f t="shared" si="5"/>
         <v>5316110.6934584752</v>
       </c>
+      <c r="R29" s="8">
+        <v>56</v>
+      </c>
+      <c r="S29" s="8">
+        <v>4380</v>
+      </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -2102,8 +4158,14 @@
         <f t="shared" si="5"/>
         <v>12234050.149260193</v>
       </c>
+      <c r="R30" s="8">
+        <v>76</v>
+      </c>
+      <c r="S30" s="8">
+        <v>5169</v>
+      </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>1</v>
       </c>
@@ -2126,8 +4188,14 @@
         <f t="shared" si="5"/>
         <v>3675875.5513617103</v>
       </c>
+      <c r="R31" s="8">
+        <v>63</v>
+      </c>
+      <c r="S31" s="8">
+        <v>4727</v>
+      </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <f>A31+1</f>
         <v>2</v>
@@ -2151,8 +4219,14 @@
         <f t="shared" si="5"/>
         <v>-773635.22054416104</v>
       </c>
+      <c r="R32" s="8">
+        <v>62</v>
+      </c>
+      <c r="S32" s="8">
+        <v>4534</v>
+      </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <f t="shared" ref="A33:A42" si="7">A32+1</f>
         <v>3</v>
@@ -2176,8 +4250,14 @@
         <f t="shared" si="5"/>
         <v>398664.26467064361</v>
       </c>
+      <c r="R33" s="8">
+        <v>53</v>
+      </c>
+      <c r="S33" s="8">
+        <v>4608</v>
+      </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <f t="shared" si="7"/>
         <v>4</v>
@@ -2201,8 +4281,14 @@
         <f t="shared" si="5"/>
         <v>3308639.257011157</v>
       </c>
+      <c r="R34" s="8">
+        <v>62</v>
+      </c>
+      <c r="S34" s="8">
+        <v>4647</v>
+      </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <f t="shared" si="7"/>
         <v>5</v>
@@ -2226,8 +4312,14 @@
         <f t="shared" si="5"/>
         <v>1775819.3471010588</v>
       </c>
+      <c r="R35" s="8">
+        <v>50</v>
+      </c>
+      <c r="S35" s="8">
+        <v>4744</v>
+      </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <f t="shared" si="7"/>
         <v>6</v>
@@ -2251,8 +4343,14 @@
         <f t="shared" si="5"/>
         <v>-2344027.2853640243</v>
       </c>
+      <c r="R36" s="8">
+        <v>51</v>
+      </c>
+      <c r="S36" s="8">
+        <v>4292</v>
+      </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <f t="shared" si="7"/>
         <v>7</v>
@@ -2276,8 +4374,14 @@
         <f t="shared" si="5"/>
         <v>-7387011.5811074525</v>
       </c>
+      <c r="R37" s="8">
+        <v>50</v>
+      </c>
+      <c r="S37" s="8">
+        <v>4349</v>
+      </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f t="shared" si="7"/>
         <v>8</v>
@@ -2301,8 +4405,14 @@
         <f t="shared" si="5"/>
         <v>-9149912.9004912656</v>
       </c>
+      <c r="R38" s="8">
+        <v>47</v>
+      </c>
+      <c r="S38" s="8">
+        <v>4297</v>
+      </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <f t="shared" si="7"/>
         <v>9</v>
@@ -2326,8 +4436,14 @@
         <f t="shared" si="5"/>
         <v>-6380149.8002379816</v>
       </c>
+      <c r="R39" s="8">
+        <v>49</v>
+      </c>
+      <c r="S39" s="8">
+        <v>4223</v>
+      </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <f>A39+1</f>
         <v>10</v>
@@ -2351,8 +4467,14 @@
         <f t="shared" si="5"/>
         <v>-565627.37157770572</v>
       </c>
+      <c r="R40" s="8">
+        <v>52</v>
+      </c>
+      <c r="S40" s="8">
+        <v>4600</v>
+      </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <f t="shared" si="7"/>
         <v>11</v>
@@ -2376,8 +4498,14 @@
         <f t="shared" si="5"/>
         <v>4823923.4912708895</v>
       </c>
+      <c r="R41" s="8">
+        <v>58</v>
+      </c>
+      <c r="S41" s="8">
+        <v>4516</v>
+      </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <f t="shared" si="7"/>
         <v>12</v>
@@ -2394,6 +4522,12 @@
       <c r="F42" s="6">
         <f>D41+E41+F30</f>
         <v>29118255.20883856</v>
+      </c>
+      <c r="R42" s="8">
+        <v>65</v>
+      </c>
+      <c r="S42" s="8">
+        <v>5544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>